<commit_message>
commit home page, shop page, not found page, product page
</commit_message>
<xml_diff>
--- a/KeHoachThucHien.xlsx
+++ b/KeHoachThucHien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HocKiI-Nam4-(22-23)\TieuLuanChuyenNganh\book_sale_online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE230A55-D0AA-4F85-A2AA-170317DB4C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D99BEA-C2CB-428A-A7B3-CF449B72F663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="8664" yWindow="5808" windowWidth="13044" windowHeight="6348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="116">
   <si>
     <t>STT</t>
   </si>
@@ -425,12 +425,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -445,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -500,6 +506,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1022,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1153,7 +1174,9 @@
       <c r="G8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="I8" s="9"/>
       <c r="J8" s="5" t="s">
         <v>80</v>
@@ -1179,25 +1202,25 @@
       <c r="I9" s="14"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="7" t="s">
+    <row r="10" spans="1:10" s="24" customFormat="1" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="15" t="s">
+      <c r="D10" s="20"/>
+      <c r="E10" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="12"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">

</xml_diff>